<commit_message>
moneybin: update RSI spreadsheet
Signed-off-by: Thiago Farina <tfransosi@gmail.com>
</commit_message>
<xml_diff>
--- a/c/apps/moneybin/OSCILLATOR-RSI.xlsx
+++ b/c/apps/moneybin/OSCILLATOR-RSI.xlsx
@@ -138,8 +138,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -175,586 +179,590 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.4591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>44308</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="3" t="n">
         <v>16.16</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="3" t="n">
         <v>16.290001</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="3" t="n">
         <v>14.88</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="3" t="n">
         <v>15.11</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="3" t="n">
         <v>15.11</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>9261600</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="2" t="n">
         <v>44309</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="3" t="n">
         <v>15.24</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="3" t="n">
         <v>16.690001</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="3" t="n">
         <v>15.19</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="3" t="n">
         <v>16.360001</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="3" t="n">
         <v>16.360001</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>10938600</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="1" t="n">
         <f aca="false">E3-E2</f>
         <v>1.250001</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3" s="1" t="n">
         <f aca="false">IF(H3&gt;0,H3, 0)</f>
         <v>1.250001</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="J3" s="1" t="n">
         <f aca="false">IF(H3&lt;0,-1 * H3, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="2" t="n">
         <v>44312</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="3" t="n">
         <v>16.629999</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="3" t="n">
         <v>17.08</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="3" t="n">
         <v>16.4</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <v>9181400</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="1" t="n">
         <f aca="false">E4-E3</f>
         <v>0.639999</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="I4" s="1" t="n">
         <f aca="false">IF(H4&gt;0,H4, 0)</f>
         <v>0.639999</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="J4" s="1" t="n">
         <f aca="false">IF(H4&lt;0,-1 * H4, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="2" t="n">
         <v>44313</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="3" t="n">
         <v>16.950001</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="3" t="n">
         <v>18.52</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="3" t="n">
         <v>16.799999</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="3" t="n">
         <v>17.940001</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="3" t="n">
         <v>17.940001</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <v>12543800</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="1" t="n">
         <f aca="false">E5-E4</f>
         <v>0.940000999999999</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="I5" s="1" t="n">
         <f aca="false">IF(H5&gt;0,H5, 0)</f>
         <v>0.940000999999999</v>
       </c>
-      <c r="J5" s="0" t="n">
+      <c r="J5" s="1" t="n">
         <f aca="false">IF(H5&lt;0,-1 * H5, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="2" t="n">
         <v>44314</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="3" t="n">
         <v>18.17</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="3" t="n">
         <v>18.48</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="3" t="n">
         <v>17.41</v>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="3" t="n">
         <v>18.200001</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="3" t="n">
         <v>18.200001</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="1" t="n">
         <v>6862500</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6" s="1" t="n">
         <f aca="false">E6-E5</f>
         <v>0.260000000000002</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="I6" s="1" t="n">
         <f aca="false">IF(H6&gt;0,H6, 0)</f>
         <v>0.260000000000002</v>
       </c>
-      <c r="J6" s="0" t="n">
+      <c r="J6" s="1" t="n">
         <f aca="false">IF(H6&lt;0,-1 * H6, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="2" t="n">
         <v>44315</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="3" t="n">
         <v>18.209999</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="3" t="n">
         <v>19.09</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="3" t="n">
         <v>17.620001</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="3" t="n">
         <v>17.870001</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="3" t="n">
         <v>17.870001</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>9836600</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7" s="1" t="n">
         <f aca="false">E7-E6</f>
         <v>-0.330000000000002</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="I7" s="1" t="n">
         <f aca="false">IF(H7&gt;0,H7, 0)</f>
         <v>0</v>
       </c>
-      <c r="J7" s="0" t="n">
+      <c r="J7" s="1" t="n">
         <f aca="false">IF(H7&lt;0,-1 * H7, 0)</f>
         <v>0.330000000000002</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="2" t="n">
         <v>44316</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="3" t="n">
         <v>17.790001</v>
       </c>
-      <c r="C8" s="2" t="n">
+      <c r="C8" s="3" t="n">
         <v>18.5</v>
       </c>
-      <c r="D8" s="2" t="n">
+      <c r="D8" s="3" t="n">
         <v>17.26</v>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="E8" s="3" t="n">
         <v>18.389999</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="3" t="n">
         <v>18.389999</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="1" t="n">
         <v>9766900</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8" s="1" t="n">
         <f aca="false">E8-E7</f>
         <v>0.519998000000001</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="I8" s="1" t="n">
         <f aca="false">IF(H8&gt;0,H8, 0)</f>
         <v>0.519998000000001</v>
       </c>
-      <c r="J8" s="0" t="n">
+      <c r="J8" s="1" t="n">
         <f aca="false">IF(H8&lt;0,-1 * H8, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="2" t="n">
         <v>44319</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="3" t="n">
         <v>18.559999</v>
       </c>
-      <c r="C9" s="2" t="n">
+      <c r="C9" s="3" t="n">
         <v>19.25</v>
       </c>
-      <c r="D9" s="2" t="n">
+      <c r="D9" s="3" t="n">
         <v>18.24</v>
       </c>
-      <c r="E9" s="2" t="n">
+      <c r="E9" s="3" t="n">
         <v>18.91</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="3" t="n">
         <v>18.902515</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <v>7035600</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9" s="1" t="n">
         <f aca="false">E9-E8</f>
         <v>0.520001000000001</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="I9" s="1" t="n">
         <f aca="false">IF(H9&gt;0,H9, 0)</f>
         <v>0.520001000000001</v>
       </c>
-      <c r="J9" s="0" t="n">
+      <c r="J9" s="1" t="n">
         <f aca="false">IF(H9&lt;0,-1 * H9, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+      <c r="A10" s="2" t="n">
         <v>44320</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="C10" s="2" t="n">
+      <c r="C10" s="3" t="n">
         <v>19.110001</v>
       </c>
-      <c r="D10" s="2" t="n">
+      <c r="D10" s="3" t="n">
         <v>18.24</v>
       </c>
-      <c r="E10" s="2" t="n">
+      <c r="E10" s="3" t="n">
         <v>18.379999</v>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="F10" s="3" t="n">
         <v>18.372725</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <v>4495700</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10" s="1" t="n">
         <f aca="false">E10-E9</f>
         <v>-0.530000999999999</v>
       </c>
-      <c r="I10" s="0" t="n">
+      <c r="I10" s="1" t="n">
         <f aca="false">IF(H10&gt;0,H10, 0)</f>
         <v>0</v>
       </c>
-      <c r="J10" s="0" t="n">
+      <c r="J10" s="1" t="n">
         <f aca="false">IF(H10&lt;0,-1 * H10, 0)</f>
         <v>0.530000999999999</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+      <c r="A11" s="2" t="n">
         <v>44321</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="3" t="n">
         <v>18.48</v>
       </c>
-      <c r="C11" s="2" t="n">
+      <c r="C11" s="3" t="n">
         <v>19.09</v>
       </c>
-      <c r="D11" s="2" t="n">
+      <c r="D11" s="3" t="n">
         <v>18.120001</v>
       </c>
-      <c r="E11" s="2" t="n">
+      <c r="E11" s="3" t="n">
         <v>19.01</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="F11" s="3" t="n">
         <v>19.01</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="1" t="n">
         <v>4288800</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="H11" s="1" t="n">
         <f aca="false">E11-E10</f>
         <v>0.630001</v>
       </c>
-      <c r="I11" s="0" t="n">
+      <c r="I11" s="1" t="n">
         <f aca="false">IF(H11&gt;0,H11, 0)</f>
         <v>0.630001</v>
       </c>
-      <c r="J11" s="0" t="n">
+      <c r="J11" s="1" t="n">
         <f aca="false">IF(H11&lt;0,-1 * H11, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+      <c r="A12" s="2" t="n">
         <v>44322</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="3" t="n">
         <v>18.98</v>
       </c>
-      <c r="C12" s="2" t="n">
+      <c r="C12" s="3" t="n">
         <v>19.49</v>
       </c>
-      <c r="D12" s="2" t="n">
+      <c r="D12" s="3" t="n">
         <v>17.84</v>
       </c>
-      <c r="E12" s="2" t="n">
+      <c r="E12" s="3" t="n">
         <v>18.08</v>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="F12" s="3" t="n">
         <v>18.08</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="1" t="n">
         <v>5505500</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H12" s="1" t="n">
         <f aca="false">E12-E11</f>
         <v>-0.930000000000003</v>
       </c>
-      <c r="I12" s="0" t="n">
+      <c r="I12" s="1" t="n">
         <f aca="false">IF(H12&gt;0,H12, 0)</f>
         <v>0</v>
       </c>
-      <c r="J12" s="0" t="n">
+      <c r="J12" s="1" t="n">
         <f aca="false">IF(H12&lt;0,-1 * H12, 0)</f>
         <v>0.930000000000003</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+      <c r="A13" s="2" t="n">
         <v>44323</v>
       </c>
-      <c r="B13" s="2" t="n">
+      <c r="B13" s="3" t="n">
         <v>18.209999</v>
       </c>
-      <c r="C13" s="2" t="n">
+      <c r="C13" s="3" t="n">
         <v>18.450001</v>
       </c>
-      <c r="D13" s="2" t="n">
+      <c r="D13" s="3" t="n">
         <v>17.9</v>
       </c>
-      <c r="E13" s="2" t="n">
+      <c r="E13" s="3" t="n">
         <v>18.27</v>
       </c>
-      <c r="F13" s="2" t="n">
+      <c r="F13" s="3" t="n">
         <v>18.27</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="1" t="n">
         <v>3004200</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="H13" s="1" t="n">
         <f aca="false">E13-E12</f>
         <v>0.190000000000001</v>
       </c>
-      <c r="I13" s="0" t="n">
+      <c r="I13" s="1" t="n">
         <f aca="false">IF(H13&gt;0,H13, 0)</f>
         <v>0.190000000000001</v>
       </c>
-      <c r="J13" s="0" t="n">
+      <c r="J13" s="1" t="n">
         <f aca="false">IF(H13&lt;0,-1 * H13, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+      <c r="A14" s="2" t="n">
         <v>44326</v>
       </c>
-      <c r="B14" s="2" t="n">
+      <c r="B14" s="3" t="n">
         <v>18.709999</v>
       </c>
-      <c r="C14" s="2" t="n">
+      <c r="C14" s="3" t="n">
         <v>18.92</v>
       </c>
-      <c r="D14" s="2" t="n">
+      <c r="D14" s="3" t="n">
         <v>17.41</v>
       </c>
-      <c r="E14" s="2" t="n">
+      <c r="E14" s="3" t="n">
         <v>17.530001</v>
       </c>
-      <c r="F14" s="2" t="n">
+      <c r="F14" s="3" t="n">
         <v>17.530001</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="1" t="n">
         <v>6622000</v>
       </c>
-      <c r="H14" s="0" t="n">
+      <c r="H14" s="1" t="n">
         <f aca="false">E14-E13</f>
         <v>-0.739999000000001</v>
       </c>
-      <c r="I14" s="0" t="n">
+      <c r="I14" s="1" t="n">
         <f aca="false">IF(H14&gt;0,H14, 0)</f>
         <v>0</v>
       </c>
-      <c r="J14" s="0" t="n">
+      <c r="J14" s="1" t="n">
         <f aca="false">IF(H14&lt;0,-1 * H14, 0)</f>
         <v>0.739999000000001</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+      <c r="A15" s="2" t="n">
         <v>44327</v>
       </c>
-      <c r="B15" s="2" t="n">
+      <c r="B15" s="3" t="n">
         <v>17.200001</v>
       </c>
-      <c r="C15" s="2" t="n">
+      <c r="C15" s="3" t="n">
         <v>17.459999</v>
       </c>
-      <c r="D15" s="2" t="n">
+      <c r="D15" s="3" t="n">
         <v>16.860001</v>
       </c>
-      <c r="E15" s="2" t="n">
+      <c r="E15" s="3" t="n">
         <v>17.280001</v>
       </c>
-      <c r="F15" s="2" t="n">
+      <c r="F15" s="3" t="n">
         <v>17.280001</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="1" t="n">
         <v>3757400</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="H15" s="1" t="n">
         <f aca="false">E15-E14</f>
         <v>-0.25</v>
       </c>
-      <c r="I15" s="0" t="n">
+      <c r="I15" s="1" t="n">
         <f aca="false">IF(H15&gt;0,H15, 0)</f>
         <v>0</v>
       </c>
-      <c r="J15" s="0" t="n">
+      <c r="J15" s="1" t="n">
         <f aca="false">IF(H15&lt;0,-1 * H15, 0)</f>
         <v>0.25</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
+      <c r="A16" s="2" t="n">
         <v>44328</v>
       </c>
-      <c r="B16" s="2" t="n">
+      <c r="B16" s="3" t="n">
         <v>17.32</v>
       </c>
-      <c r="C16" s="2" t="n">
+      <c r="C16" s="3" t="n">
         <v>17.940001</v>
       </c>
-      <c r="D16" s="2" t="n">
+      <c r="D16" s="3" t="n">
         <v>16.76</v>
       </c>
-      <c r="E16" s="2" t="n">
+      <c r="E16" s="3" t="n">
         <v>16.91</v>
       </c>
-      <c r="F16" s="2" t="n">
+      <c r="F16" s="3" t="n">
         <v>16.91</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="1" t="n">
         <v>5060800</v>
       </c>
-      <c r="H16" s="0" t="n">
+      <c r="H16" s="1" t="n">
         <f aca="false">E16-E15</f>
         <v>-0.370000999999998</v>
       </c>
-      <c r="I16" s="0" t="n">
+      <c r="I16" s="1" t="n">
         <f aca="false">IF(H16&gt;0,H16, 0)</f>
         <v>0</v>
       </c>
-      <c r="J16" s="0" t="n">
+      <c r="J16" s="1" t="n">
         <f aca="false">IF(H16&lt;0,-1 * H16, 0)</f>
         <v>0.370000999999998</v>
       </c>
-      <c r="K16" s="0" t="n">
+      <c r="K16" s="1" t="n">
         <f aca="false">AVERAGE(I3:I16)</f>
         <v>0.3535715</v>
       </c>
-      <c r="L16" s="0" t="n">
+      <c r="L16" s="1" t="n">
         <f aca="false">AVERAGE(J3:J16)</f>
         <v>0.225000071428572</v>
       </c>
-      <c r="M16" s="0" t="n">
+      <c r="M16" s="1" t="n">
         <f aca="false">K16/L16</f>
         <v>1.57142839002273</v>
       </c>
-      <c r="N16" s="0" t="n">
+      <c r="N16" s="1" t="n">
         <f aca="false">IF(L16=0,100, 100-(100/(1+M16)))</f>
         <v>61.1111083676276</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I17" s="0" t="n">
+      <c r="I17" s="1" t="n">
         <f aca="false">SUM(I3:I16)</f>
         <v>4.950001</v>
       </c>
-      <c r="J17" s="0" t="n">
+      <c r="J17" s="1" t="n">
         <f aca="false">SUM(J3:J16)</f>
         <v>3.150001</v>
       </c>

</xml_diff>